<commit_message>
Adresser le top 10 OWASP
</commit_message>
<xml_diff>
--- a/revue_securite_todolist_graphql.xlsx
+++ b/revue_securite_todolist_graphql.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0-AUTO-FORMATIONS\0-PROJET\0-PROJETS_FORMATIONS_SIMPLONS\5-Cybersecurite\cours-18-19-02-2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\logiciels\xampp\htdocs\Simplon\1-cybersecurite\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383EC2F1-6B74-47D9-AF01-B14134495620}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36F6631-8846-452B-AC98-A58D4015BAB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TodoList-Graphql-backend" sheetId="1" r:id="rId1"/>
     <sheet name="Todolist-Graphql-frontend" sheetId="2" r:id="rId2"/>
+    <sheet name="OWASP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="82">
   <si>
     <t>Catégorie</t>
   </si>
@@ -185,13 +186,100 @@
   </si>
   <si>
     <t>Authentification via JWT (Bearer Token)</t>
+  </si>
+  <si>
+    <t>OWASP</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Injection</t>
+  </si>
+  <si>
+    <t>Broken Authentication.</t>
+  </si>
+  <si>
+    <t>Sensitive Data Exposure.</t>
+  </si>
+  <si>
+    <t>XML External Entities (XXE).</t>
+  </si>
+  <si>
+    <t>Broken Access Control.</t>
+  </si>
+  <si>
+    <t>Security Misconfiguration</t>
+  </si>
+  <si>
+    <t>Cross-Site Scripting (XSS)</t>
+  </si>
+  <si>
+    <t>Insecure Deserialization</t>
+  </si>
+  <si>
+    <t>Using Components with Known Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Insufficient Logging &amp; Monitoring</t>
+  </si>
+  <si>
+    <t>Des failles d'injection, telles que l'injection SQL, NoSQL, OS et LDAP, se produisent lorsque des données non approuvées sont envoyées à un interpréteur dans le cadre d'une commande ou d'une requête. Les données hostiles de l'attaquant peuvent inciter l'interpréteur à exécuter des commandes involontaires ou à accéder aux données sans autorisation appropriée.</t>
+  </si>
+  <si>
+    <t>Les fonctions applicatives liées à l'authentification et à la gestion de session sont souvent mal implémentées, ce qui permet aux attaquants de compromettre les mots de passe, les clés ou les jetons de session, ou d'exploiter d'autres failles d'implémentation pour assumer temporairement ou définitivement l'identité des autres utilisateurs</t>
+  </si>
+  <si>
+    <t>De nombreuses applications Web et API ne protègent pas correctement les données sensibles, telles que les données financières, les soins de santé et les informations personnelles. Les attaquants peuvent voler ou modifier ces données faiblement protégées pour mener une fraude par carte de crédit, un vol d'identité ou d'autres crimes. Les données sensibles peuvent être compromises sans protection supplémentaire, telle que le cryptage au repos ou en transit, et nécessitent des précautions particulières lorsqu'elles sont échangées avec le navigateur.</t>
+  </si>
+  <si>
+    <t>De nombreux processeurs XML plus anciens ou mal configurés évaluent les références d'entités externes dans les documents XML. Les entités externes peuvent être utilisées pour divulguer des fichiers internes à l'aide du gestionnaire d'URI de fichier, des partages de fichiers internes, de l'analyse des ports internes, de l'exécution de code à distance et des attaques par déni de service.</t>
+  </si>
+  <si>
+    <t>Les restrictions sur ce que les utilisateurs authentifiés sont autorisés à faire ne sont souvent pas correctement appliquées. Les attaquants peuvent exploiter ces failles pour accéder à des fonctionnalités et / ou des données non autorisées, telles que l'accès aux comptes d'autres utilisateurs, afficher des fichiers sensibles, modifier les données d'autres utilisateurs, modifier les droits d'accès, etc.</t>
+  </si>
+  <si>
+    <t>Une mauvaise configuration de la sécurité est le problème le plus courant. Ceci est généralement le résultat de configurations par défaut non sécurisées, de configurations incomplètes ou ad hoc, d'un stockage en nuage ouvert, d'en-têtes HTTP mal configurés et de messages d'erreur détaillés contenant des informations sensibles. Non seulement tous les systèmes d'exploitation, frameworks, bibliothèques et applications doivent être configurés de manière sécurisée, mais ils doivent être corrigés / mis à niveau en temps opportun.</t>
+  </si>
+  <si>
+    <t>Des failles XSS se produisent chaque fois qu'une application inclut des données non approuvées dans une nouvelle page Web sans validation ou échappement appropriée, ou met à jour une page Web existante avec des données fournies par l'utilisateur à l'aide d'une API de navigateur qui peut créer du HTML ou du JavaScript. XSS permet aux attaquants d'exécuter des scripts dans le navigateur de la victime qui peuvent détourner les sessions des utilisateurs, déformer les sites Web ou rediriger l'utilisateur vers des sites malveillants.</t>
+  </si>
+  <si>
+    <t>Une désérialisation non sécurisée conduit souvent à l'exécution de code à distance. Même si les failles de désérialisation n'entraînent pas l'exécution de code à distance, elles peuvent être utilisées pour effectuer des attaques, y compris des attaques de relecture, des attaques par injection et des attaques par élévation de privilèges.</t>
+  </si>
+  <si>
+    <t>Les composants, tels que les bibliothèques, les frameworks et d'autres modules logiciels, s'exécutent avec les mêmes privilèges que l'application. Si un composant vulnérable est exploité, une telle attaque peut faciliter de graves pertes de données ou une prise de contrôle du serveur. Les applications et les API utilisant des composants avec des vulnérabilités connues peuvent saper les défenses des applications et permettre diverses attaques et impacts.</t>
+  </si>
+  <si>
+    <t>Une journalisation et une surveillance insuffisantes, associées à une intégration manquante ou inefficace avec la réponse aux incidents, permettent aux attaquants d'attaquer davantage les systèmes, de maintenir la persistance, de basculer vers plus de systèmes et de falsifier, extraire ou détruire les données. La plupart des études sur les violations montrent que le délai de détection d'une violation est supérieur à 200 jours, généralement détecté par des parties externes plutôt que par des processus ou une surveillance internes.</t>
+  </si>
+  <si>
+    <t>ORM</t>
+  </si>
+  <si>
+    <t>Utilisation de l'ORM eloquent de Laravel</t>
+  </si>
+  <si>
+    <t>Injection.</t>
+  </si>
+  <si>
+    <t>Injection / Cross-Site Scripting (XSS) / Insecure Deserialization.</t>
+  </si>
+  <si>
+    <t>https://owasp.org/www-project-top-ten/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +291,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -246,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -297,11 +393,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,8 +480,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -631,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,9 +815,10 @@
     <col min="3" max="3" width="24.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="54.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -659,11 +831,14 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>51</v>
       </c>
@@ -676,11 +851,14 @@
       <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -693,11 +871,14 @@
       <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="25">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -710,11 +891,14 @@
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -727,11 +911,14 @@
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -744,11 +931,14 @@
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -761,11 +951,14 @@
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -778,11 +971,14 @@
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -795,11 +991,14 @@
       <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -812,11 +1011,14 @@
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -829,11 +1031,14 @@
       <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -846,11 +1051,14 @@
       <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -863,11 +1071,14 @@
       <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -880,11 +1091,14 @@
       <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -897,11 +1111,14 @@
       <c r="D15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -914,11 +1131,14 @@
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -931,11 +1151,14 @@
       <c r="D17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -948,11 +1171,14 @@
       <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -965,11 +1191,14 @@
       <c r="D19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
@@ -982,11 +1211,14 @@
       <c r="D20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -999,11 +1231,12 @@
       <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1016,11 +1249,14 @@
       <c r="D22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1033,11 +1269,14 @@
       <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1050,11 +1289,12 @@
       <c r="D24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
@@ -1067,11 +1307,14 @@
       <c r="D25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
@@ -1084,11 +1327,14 @@
       <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>22</v>
       </c>
@@ -1101,11 +1347,14 @@
       <c r="D27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
@@ -1118,11 +1367,14 @@
       <c r="D28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>48</v>
       </c>
@@ -1135,11 +1387,14 @@
       <c r="D29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
@@ -1152,8 +1407,31 @@
       <c r="D30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="26">
         <v>5</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3">
+        <v>5</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1164,22 +1442,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CABCEDC-40FF-489E-8356-8AB498064FA5}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="114.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.21875" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1195,8 +1474,11 @@
       <c r="E1" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -1209,11 +1491,14 @@
       <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="25">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1226,11 +1511,14 @@
       <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1243,11 +1531,14 @@
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>44</v>
       </c>
@@ -1260,11 +1551,14 @@
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>46</v>
       </c>
@@ -1277,74 +1571,77 @@
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -1431,4 +1728,157 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA761FE-BE1C-444B-BC68-81E772D244F3}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="44.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="131.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>8</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{3D37EEC0-1B5B-4018-AF88-6514767D15C0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>